<commit_message>
nye billeder og lidt godt
</commit_message>
<xml_diff>
--- a/Makroøkonomisk projekt.xlsx
+++ b/Makroøkonomisk projekt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aaudk-my.sharepoint.com/personal/ci65gm_student_aau_dk/Documents/Økonomi/4. semester/Projekt/projekteksamen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1081" documentId="11_9C5455BF84DCCE936262E6F99831F45BBA780A8F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C46C8B20-2392-8540-A3C7-FB6152DE418A}"/>
+  <xr:revisionPtr revIDLastSave="1082" documentId="11_9C5455BF84DCCE936262E6F99831F45BBA780A8F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABC999FB-0BDF-1749-B79F-D3523E84BC2A}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="112">
   <si>
     <t>Date</t>
   </si>
@@ -421,9 +421,6 @@
   </si>
   <si>
     <t>Generel government net lending/borrowing for EU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Debt brake </t>
   </si>
 </sst>
 </file>
@@ -895,10 +892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AS289"/>
+  <dimension ref="A1:AP289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF72" zoomScale="106" workbookViewId="0">
-      <selection activeCell="AW92" sqref="AW92"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="AS11" sqref="AS11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -925,7 +922,7 @@
     <col min="45" max="45" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -992,11 +989,8 @@
       <c r="AP1" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="AS1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>36526</v>
       </c>
@@ -1062,11 +1056,8 @@
       <c r="AP2" s="21">
         <v>8.6999999999999993</v>
       </c>
-      <c r="AS2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>36617</v>
       </c>
@@ -1132,11 +1123,8 @@
       <c r="AP3" s="21">
         <v>9.1</v>
       </c>
-      <c r="AS3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>36708</v>
       </c>
@@ -1202,11 +1190,8 @@
       <c r="AP4" s="21">
         <v>8.8000000000000007</v>
       </c>
-      <c r="AS4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>36800</v>
       </c>
@@ -1272,11 +1257,8 @@
       <c r="AP5" s="21">
         <v>7.5</v>
       </c>
-      <c r="AS5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>36892</v>
       </c>
@@ -1342,11 +1324,8 @@
       <c r="AP6" s="21">
         <v>9.5</v>
       </c>
-      <c r="AS6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>36982</v>
       </c>
@@ -1412,11 +1391,8 @@
       <c r="AP7" s="21">
         <v>8.6</v>
       </c>
-      <c r="AS7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>37073</v>
       </c>
@@ -1482,11 +1458,8 @@
       <c r="AP8" s="21">
         <v>8</v>
       </c>
-      <c r="AS8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>37165</v>
       </c>
@@ -1552,11 +1525,8 @@
       <c r="AP9" s="21">
         <v>7.5</v>
       </c>
-      <c r="AS9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>37257</v>
       </c>
@@ -1622,11 +1592,8 @@
       <c r="AP10" s="21">
         <v>8.9</v>
       </c>
-      <c r="AS10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>37347</v>
       </c>
@@ -1691,11 +1658,8 @@
       <c r="AP11" s="21">
         <v>8.8000000000000007</v>
       </c>
-      <c r="AS11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>37438</v>
       </c>
@@ -1761,11 +1725,8 @@
       <c r="AP12" s="21">
         <v>9.6</v>
       </c>
-      <c r="AS12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>37530</v>
       </c>
@@ -1831,11 +1792,8 @@
       <c r="AP13" s="21">
         <v>9.1</v>
       </c>
-      <c r="AS13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>37622</v>
       </c>
@@ -1901,11 +1859,8 @@
       <c r="AP14" s="21">
         <v>11.1</v>
       </c>
-      <c r="AS14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>37712</v>
       </c>
@@ -1971,11 +1926,8 @@
       <c r="AP15" s="21">
         <v>9.1</v>
       </c>
-      <c r="AS15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>37803</v>
       </c>
@@ -2041,11 +1993,8 @@
       <c r="AP16" s="21">
         <v>10</v>
       </c>
-      <c r="AS16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>37895</v>
       </c>
@@ -2111,11 +2060,8 @@
       <c r="AP17" s="21">
         <v>10</v>
       </c>
-      <c r="AS17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>37987</v>
       </c>
@@ -2181,11 +2127,8 @@
       <c r="AP18" s="21">
         <v>10.6</v>
       </c>
-      <c r="AS18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>38078</v>
       </c>
@@ -2251,11 +2194,8 @@
       <c r="AP19" s="21">
         <v>11.6</v>
       </c>
-      <c r="AS19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>38169</v>
       </c>
@@ -2321,11 +2261,8 @@
       <c r="AP20" s="21">
         <v>9.8000000000000007</v>
       </c>
-      <c r="AS20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>38261</v>
       </c>
@@ -2391,11 +2328,8 @@
       <c r="AP21" s="21">
         <v>8.8000000000000007</v>
       </c>
-      <c r="AS21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>38353</v>
       </c>
@@ -2461,11 +2395,8 @@
       <c r="AP22" s="21">
         <v>11.1</v>
       </c>
-      <c r="AS22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>38443</v>
       </c>
@@ -2531,11 +2462,8 @@
       <c r="AP23" s="21">
         <v>11.1</v>
       </c>
-      <c r="AS23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:45" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>38534</v>
       </c>
@@ -2600,11 +2528,8 @@
       <c r="AP24" s="21">
         <v>10.8</v>
       </c>
-      <c r="AS24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>38626</v>
       </c>
@@ -2669,11 +2594,8 @@
       <c r="AP25" s="21">
         <v>12.4</v>
       </c>
-      <c r="AS25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>38718</v>
       </c>
@@ -2738,11 +2660,8 @@
       <c r="AP26" s="21">
         <v>12.5</v>
       </c>
-      <c r="AS26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>38808</v>
       </c>
@@ -2807,11 +2726,8 @@
       <c r="AP27" s="21">
         <v>13.7</v>
       </c>
-      <c r="AS27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>38899</v>
       </c>
@@ -2876,11 +2792,8 @@
       <c r="AP28" s="21">
         <v>12.2</v>
       </c>
-      <c r="AS28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>38991</v>
       </c>
@@ -2945,11 +2858,8 @@
       <c r="AP29" s="21">
         <v>12.5</v>
       </c>
-      <c r="AS29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>39083</v>
       </c>
@@ -3014,11 +2924,8 @@
       <c r="AP30" s="21">
         <v>13.8</v>
       </c>
-      <c r="AS30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>39173</v>
       </c>
@@ -3083,11 +2990,8 @@
       <c r="AP31" s="21">
         <v>15</v>
       </c>
-      <c r="AS31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>39264</v>
       </c>
@@ -3152,11 +3056,8 @@
       <c r="AP32" s="21">
         <v>14.3</v>
       </c>
-      <c r="AS32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>39356</v>
       </c>
@@ -3221,11 +3122,8 @@
       <c r="AP33" s="21">
         <v>13.9</v>
       </c>
-      <c r="AS33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>39448</v>
       </c>
@@ -3290,11 +3188,8 @@
       <c r="AP34" s="21">
         <v>11.5</v>
       </c>
-      <c r="AS34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>39539</v>
       </c>
@@ -3359,11 +3254,8 @@
       <c r="AP35" s="21">
         <v>10.9</v>
       </c>
-      <c r="AS35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>39630</v>
       </c>
@@ -3428,11 +3320,8 @@
       <c r="AP36" s="21">
         <v>9.5</v>
       </c>
-      <c r="AS36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>39722</v>
       </c>
@@ -3497,11 +3386,8 @@
       <c r="AP37" s="21">
         <v>7.1</v>
       </c>
-      <c r="AS37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>39814</v>
       </c>
@@ -3566,11 +3452,8 @@
       <c r="AP38" s="21">
         <v>6.4</v>
       </c>
-      <c r="AS38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>39904</v>
       </c>
@@ -3635,11 +3518,8 @@
       <c r="AP39" s="21">
         <v>8.1999999999999993</v>
       </c>
-      <c r="AS39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>39995</v>
       </c>
@@ -3704,11 +3584,8 @@
       <c r="AP40" s="21">
         <v>10.6</v>
       </c>
-      <c r="AS40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>40087</v>
       </c>
@@ -3773,11 +3650,8 @@
       <c r="AP41" s="21">
         <v>11.9</v>
       </c>
-      <c r="AS41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>40179</v>
       </c>
@@ -3842,11 +3716,8 @@
       <c r="AP42" s="21">
         <v>12.2</v>
       </c>
-      <c r="AS42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>40269</v>
       </c>
@@ -3911,11 +3782,8 @@
       <c r="AP43" s="21">
         <v>10.8</v>
       </c>
-      <c r="AS43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>40360</v>
       </c>
@@ -3980,11 +3848,8 @@
       <c r="AP44" s="21">
         <v>9.9</v>
       </c>
-      <c r="AS44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>40452</v>
       </c>
@@ -4049,11 +3914,8 @@
       <c r="AP45" s="21">
         <v>9.9</v>
       </c>
-      <c r="AS45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>40544</v>
       </c>
@@ -4118,11 +3980,8 @@
       <c r="AP46" s="21">
         <v>10.199999999999999</v>
       </c>
-      <c r="AS46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>40634</v>
       </c>
@@ -4187,11 +4046,8 @@
       <c r="AP47" s="21">
         <v>10</v>
       </c>
-      <c r="AS47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>40725</v>
       </c>
@@ -4256,11 +4112,8 @@
       <c r="AP48" s="21">
         <v>9.4</v>
       </c>
-      <c r="AS48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>40817</v>
       </c>
@@ -4325,11 +4178,8 @@
       <c r="AP49" s="21">
         <v>8.8000000000000007</v>
       </c>
-      <c r="AS49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>40909</v>
       </c>
@@ -4394,11 +4244,8 @@
       <c r="AP50" s="21">
         <v>8.1</v>
       </c>
-      <c r="AS50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>41000</v>
       </c>
@@ -4463,11 +4310,8 @@
       <c r="AP51" s="21">
         <v>7.7</v>
       </c>
-      <c r="AS51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>41091</v>
       </c>
@@ -4532,11 +4376,8 @@
       <c r="AP52" s="21">
         <v>7.5</v>
       </c>
-      <c r="AS52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>41183</v>
       </c>
@@ -4601,11 +4442,8 @@
       <c r="AP53" s="21">
         <v>8.1</v>
       </c>
-      <c r="AS53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>41275</v>
       </c>
@@ -4670,11 +4508,8 @@
       <c r="AP54" s="21">
         <v>7.9</v>
       </c>
-      <c r="AS54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>41365</v>
       </c>
@@ -4739,11 +4574,8 @@
       <c r="AP55" s="21">
         <v>7.6</v>
       </c>
-      <c r="AS55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>41456</v>
       </c>
@@ -4808,11 +4640,8 @@
       <c r="AP56" s="21">
         <v>7.9</v>
       </c>
-      <c r="AS56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>41548</v>
       </c>
@@ -4877,11 +4706,8 @@
       <c r="AP57" s="21">
         <v>7.7</v>
       </c>
-      <c r="AS57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>41640</v>
       </c>
@@ -4946,11 +4772,8 @@
       <c r="AP58" s="21">
         <v>7.5</v>
       </c>
-      <c r="AS58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>41730</v>
       </c>
@@ -5015,11 +4838,8 @@
       <c r="AP59" s="21">
         <v>7.6</v>
       </c>
-      <c r="AS59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>41821</v>
       </c>
@@ -5084,11 +4904,8 @@
       <c r="AP60" s="21">
         <v>7.2</v>
       </c>
-      <c r="AS60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>41913</v>
       </c>
@@ -5153,11 +4970,8 @@
       <c r="AP61" s="21">
         <v>7.3</v>
       </c>
-      <c r="AS61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>42005</v>
       </c>
@@ -5222,11 +5036,8 @@
       <c r="AP62" s="21">
         <v>7.1</v>
       </c>
-      <c r="AS62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>42095</v>
       </c>
@@ -5291,11 +5102,8 @@
       <c r="AP63" s="21">
         <v>7.1</v>
       </c>
-      <c r="AS63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>42186</v>
       </c>
@@ -5360,11 +5168,8 @@
       <c r="AP64" s="21">
         <v>7</v>
       </c>
-      <c r="AS64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>42278</v>
       </c>
@@ -5429,11 +5234,8 @@
       <c r="AP65" s="21">
         <v>6.9</v>
       </c>
-      <c r="AS65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>42370</v>
       </c>
@@ -5498,11 +5300,8 @@
       <c r="AP66" s="21">
         <v>6.9</v>
       </c>
-      <c r="AS66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>42461</v>
       </c>
@@ -5567,11 +5366,8 @@
       <c r="AP67" s="21">
         <v>6.8</v>
       </c>
-      <c r="AS67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>42552</v>
       </c>
@@ -5636,11 +5432,8 @@
       <c r="AP68" s="21">
         <v>6.8</v>
       </c>
-      <c r="AS68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>42644</v>
       </c>
@@ -5705,11 +5498,8 @@
       <c r="AP69" s="21">
         <v>6.9</v>
       </c>
-      <c r="AS69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>42736</v>
       </c>
@@ -5774,11 +5564,8 @@
       <c r="AP70" s="21">
         <v>7</v>
       </c>
-      <c r="AS70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>42826</v>
       </c>
@@ -5843,11 +5630,8 @@
       <c r="AP71" s="21">
         <v>7</v>
       </c>
-      <c r="AS71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>42917</v>
       </c>
@@ -5912,11 +5696,8 @@
       <c r="AP72" s="21">
         <v>6.9</v>
       </c>
-      <c r="AS72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>43009</v>
       </c>
@@ -5981,11 +5762,8 @@
       <c r="AP73" s="21">
         <v>6.8</v>
       </c>
-      <c r="AS73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>43101</v>
       </c>
@@ -6050,11 +5828,8 @@
       <c r="AP74" s="21">
         <v>6.9</v>
       </c>
-      <c r="AS74">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>43191</v>
       </c>
@@ -6119,11 +5894,8 @@
       <c r="AP75" s="21">
         <v>6.9</v>
       </c>
-      <c r="AS75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>43282</v>
       </c>
@@ -6188,11 +5960,8 @@
       <c r="AP76" s="21">
         <v>6.7</v>
       </c>
-      <c r="AS76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>43374</v>
       </c>
@@ -6257,11 +6026,8 @@
       <c r="AP77" s="21">
         <v>6.5</v>
       </c>
-      <c r="AS77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>43466</v>
       </c>
@@ -6326,11 +6092,8 @@
       <c r="AP78" s="21">
         <v>6.3</v>
       </c>
-      <c r="AS78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>43556</v>
       </c>
@@ -6395,11 +6158,8 @@
       <c r="AP79" s="21">
         <v>6</v>
       </c>
-      <c r="AS79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>43647</v>
       </c>
@@ -6464,11 +6224,8 @@
       <c r="AP80" s="21">
         <v>5.9</v>
       </c>
-      <c r="AS80">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>43739</v>
       </c>
@@ -6533,11 +6290,8 @@
       <c r="AP81" s="21">
         <v>5.8</v>
       </c>
-      <c r="AS81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>43831</v>
       </c>
@@ -6602,11 +6356,8 @@
       <c r="AP82" s="21">
         <v>-6.9</v>
       </c>
-      <c r="AS82">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>43922</v>
       </c>
@@ -6671,11 +6422,8 @@
       <c r="AP83" s="21">
         <v>3.1</v>
       </c>
-      <c r="AS83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>44013</v>
       </c>
@@ -6740,11 +6488,8 @@
       <c r="AP84" s="21">
         <v>4.8</v>
       </c>
-      <c r="AS84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>44105</v>
       </c>
@@ -6809,11 +6554,8 @@
       <c r="AP85" s="21">
         <v>6.4</v>
       </c>
-      <c r="AS85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>44197</v>
       </c>
@@ -6878,11 +6620,8 @@
       <c r="AP86" s="21">
         <v>18.7</v>
       </c>
-      <c r="AS86">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="87" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>44287</v>
       </c>
@@ -6947,11 +6686,8 @@
       <c r="AP87" s="21">
         <v>8.3000000000000007</v>
       </c>
-      <c r="AS87">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>44378</v>
       </c>
@@ -7016,11 +6752,8 @@
       <c r="AP88" s="21">
         <v>5.2</v>
       </c>
-      <c r="AS88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>44470</v>
       </c>
@@ -7085,11 +6818,8 @@
       <c r="AP89" s="21">
         <v>4.3</v>
       </c>
-      <c r="AS89">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="90" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>44562</v>
       </c>
@@ -7154,11 +6884,8 @@
       <c r="AP90" s="21">
         <v>4.8</v>
       </c>
-      <c r="AS90">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>44652</v>
       </c>
@@ -7223,11 +6950,8 @@
       <c r="AP91" s="21">
         <v>0.4</v>
       </c>
-      <c r="AS91">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>44743</v>
       </c>
@@ -7292,11 +7016,8 @@
       <c r="AP92" s="21">
         <v>3.9</v>
       </c>
-      <c r="AS92">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>44835</v>
       </c>
@@ -7361,11 +7082,8 @@
       <c r="AP93" s="21">
         <v>2.9</v>
       </c>
-      <c r="AS93">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>44927</v>
       </c>
@@ -7426,11 +7144,8 @@
       <c r="AP94" s="21">
         <v>4.5</v>
       </c>
-      <c r="AS94">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="95" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>45017</v>
       </c>
@@ -7491,11 +7206,8 @@
       <c r="AP95" s="21">
         <v>6.3</v>
       </c>
-      <c r="AS95">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="96" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>45108</v>
       </c>
@@ -7553,11 +7265,8 @@
       <c r="AP96" s="21">
         <v>4.9000000000000004</v>
       </c>
-      <c r="AS96">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="97" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>45200</v>
       </c>
@@ -7604,11 +7313,8 @@
       <c r="AP97" s="21">
         <v>5.2</v>
       </c>
-      <c r="AS97">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="98" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D98" s="1"/>
       <c r="I98" s="19"/>
       <c r="AG98" s="21">
@@ -7626,60 +7332,57 @@
       <c r="AP98" s="21">
         <v>5.3</v>
       </c>
-      <c r="AS98">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:45" x14ac:dyDescent="0.2">
+    </row>
+    <row r="99" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D99" s="1"/>
       <c r="I99" s="19"/>
     </row>
-    <row r="100" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D100" s="1"/>
       <c r="I100" s="19"/>
     </row>
-    <row r="101" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D101" s="1"/>
       <c r="I101" s="19"/>
     </row>
-    <row r="102" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D102" s="1"/>
       <c r="I102" s="19"/>
     </row>
-    <row r="103" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D103" s="1"/>
       <c r="I103" s="19"/>
     </row>
-    <row r="104" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D104" s="1"/>
       <c r="I104" s="19"/>
     </row>
-    <row r="105" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D105" s="1"/>
       <c r="I105" s="19"/>
     </row>
-    <row r="106" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D106" s="1"/>
       <c r="I106" s="19"/>
     </row>
-    <row r="107" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D107" s="1"/>
       <c r="I107" s="19"/>
     </row>
-    <row r="108" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:42" x14ac:dyDescent="0.2">
       <c r="D108" s="1"/>
       <c r="I108" s="19"/>
     </row>
-    <row r="109" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:42" x14ac:dyDescent="0.2">
       <c r="I109" s="19"/>
     </row>
-    <row r="110" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:42" x14ac:dyDescent="0.2">
       <c r="I110" s="19"/>
     </row>
-    <row r="111" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:42" x14ac:dyDescent="0.2">
       <c r="I111" s="19"/>
     </row>
-    <row r="112" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:42" x14ac:dyDescent="0.2">
       <c r="I112" s="19"/>
     </row>
     <row r="113" spans="9:9" x14ac:dyDescent="0.2">

</xml_diff>